<commit_message>
clear_contents instead of delete cells when shrinking tables via table.update()
</commit_message>
<xml_diff>
--- a/tests/tables.xlsx
+++ b/tests/tables.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10502"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/fz/dev/xlwings/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A88D045-8897-E747-B4C6-278F0FED0425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A632F7-C6C3-A64E-96C0-ADAC17D3340E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3960" yWindow="-21140" windowWidth="19200" windowHeight="21140" xr2:uid="{2B61329F-6E4C-5D40-BD15-3675A807F94C}"/>
+    <workbookView xWindow="-3960" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{2B61329F-6E4C-5D40-BD15-3675A807F94C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="template" sheetId="1" r:id="rId1"/>
     <sheet name="expected" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{2F53F9B3-2C49-B84F-8CE6-10633FF858E6}" name="Table715" displayName="Table715" ref="A24:E28" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{2F53F9B3-2C49-B84F-8CE6-10633FF858E6}" name="Table715" displayName="Table715" ref="A39:E43" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C3E69330-0F67-3F4F-B3DB-46BB1A09657F}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{6D292AC5-FCC7-D944-B38F-6BAE38D00B7A}" name="Column2"/>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B5907D2F-F52A-CC4D-A9DB-36CDE7DC37AD}" name="Table1116" displayName="Table1116" ref="A37:D41" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B5907D2F-F52A-CC4D-A9DB-36CDE7DC37AD}" name="Table1116" displayName="Table1116" ref="A52:D56" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{304ABC6E-E80A-084E-BBEF-77924CD89712}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{FEADA174-11D6-5C45-BDE6-E36EBD522E94}" name="Column2"/>
@@ -589,10 +589,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABE0211-3F53-7143-A88B-6E57FE83243B}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -801,158 +801,158 @@
         <v>5555</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
         <v>0</v>
       </c>
-      <c r="B24">
+      <c r="B39">
         <v>1</v>
       </c>
-      <c r="C24">
+      <c r="C39">
         <v>11</v>
       </c>
-      <c r="D24">
+      <c r="D39">
         <v>111</v>
       </c>
-      <c r="E24">
+      <c r="E39">
         <v>1111</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>1</v>
       </c>
-      <c r="B25">
+      <c r="B40">
         <v>2</v>
       </c>
-      <c r="C25">
+      <c r="C40">
         <v>22</v>
       </c>
-      <c r="D25">
+      <c r="D40">
         <v>222</v>
       </c>
-      <c r="E25">
+      <c r="E40">
         <v>2222</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>2</v>
       </c>
-      <c r="B26">
+      <c r="B41">
         <v>3</v>
       </c>
-      <c r="C26">
+      <c r="C41">
         <v>33</v>
       </c>
-      <c r="D26">
+      <c r="D41">
         <v>333</v>
       </c>
-      <c r="E26">
+      <c r="E41">
         <v>3333</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
         <v>3</v>
       </c>
-      <c r="B27">
+      <c r="B42">
         <v>4</v>
       </c>
-      <c r="C27">
+      <c r="C42">
         <v>44</v>
       </c>
-      <c r="D27">
+      <c r="D42">
         <v>444</v>
       </c>
-      <c r="E27">
+      <c r="E42">
         <v>4444</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
         <v>4</v>
       </c>
-      <c r="B28">
+      <c r="B43">
         <v>5</v>
       </c>
-      <c r="C28">
+      <c r="C43">
         <v>55</v>
       </c>
-      <c r="D28">
+      <c r="D43">
         <v>555</v>
       </c>
-      <c r="E28">
+      <c r="E43">
         <v>5555</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
         <v>1</v>
       </c>
-      <c r="B37">
+      <c r="B52">
         <v>11</v>
       </c>
-      <c r="C37">
+      <c r="C52">
         <v>111</v>
       </c>
-      <c r="D37">
+      <c r="D52">
         <v>1111</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
         <v>2</v>
       </c>
-      <c r="B38">
+      <c r="B53">
         <v>22</v>
       </c>
-      <c r="C38">
+      <c r="C53">
         <v>222</v>
       </c>
-      <c r="D38">
+      <c r="D53">
         <v>2222</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
         <v>3</v>
       </c>
-      <c r="B39">
+      <c r="B54">
         <v>33</v>
       </c>
-      <c r="C39">
+      <c r="C54">
         <v>333</v>
       </c>
-      <c r="D39">
+      <c r="D54">
         <v>3333</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
         <v>4</v>
       </c>
-      <c r="B40">
+      <c r="B55">
         <v>44</v>
       </c>
-      <c r="C40">
+      <c r="C55">
         <v>444</v>
       </c>
-      <c r="D40">
+      <c r="D55">
         <v>4444</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
         <v>5</v>
       </c>
-      <c r="B41">
+      <c r="B56">
         <v>55</v>
       </c>
-      <c r="C41">
+      <c r="C56">
         <v>555</v>
       </c>
-      <c r="D41">
+      <c r="D56">
         <v>5555</v>
       </c>
     </row>

</xml_diff>